<commit_message>
create api for get profile details
</commit_message>
<xml_diff>
--- a/app/public/excel/Book1.xlsx
+++ b/app/public/excel/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -84,9 +84,6 @@
     <t>React js</t>
   </si>
   <si>
-    <t>23/11/1997</t>
-  </si>
-  <si>
     <t>sukhvirsingh.ameotech@gmail.com</t>
   </si>
   <si>
@@ -130,6 +127,45 @@
   </si>
   <si>
     <t>Dist. - Palampur</t>
+  </si>
+  <si>
+    <t>Varun Gautam</t>
+  </si>
+  <si>
+    <t>varungautam.ameotech@gmail.com</t>
+  </si>
+  <si>
+    <t>varun_ameotech</t>
+  </si>
+  <si>
+    <t>Sr. Full Stack Developer</t>
+  </si>
+  <si>
+    <t>Dot Net Developer</t>
+  </si>
+  <si>
+    <t>City: - Kurali</t>
+  </si>
+  <si>
+    <t>Hr Department</t>
+  </si>
+  <si>
+    <t>hr@ameotech.gmail.com</t>
+  </si>
+  <si>
+    <t>hr_admin</t>
+  </si>
+  <si>
+    <t>HrAdmin@123</t>
+  </si>
+  <si>
+    <t>Hr Manager</t>
+  </si>
+  <si>
+    <t>HRM</t>
+  </si>
+  <si>
+    <t>moderator</t>
   </si>
 </sst>
 </file>
@@ -484,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -577,8 +613,9 @@
       <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="3">
-        <v>44594</v>
+      <c r="H2" s="3" t="e">
+        <f>DATEVALUE(2/3/2022)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>17</v>
@@ -587,10 +624,11 @@
         <v>10000</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="N2" s="3" t="e">
+        <f>DATEVALUE(11/23/1997)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -598,10 +636,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D3" s="1">
         <v>123456</v>
@@ -610,13 +648,14 @@
         <v>9087654324</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="3">
-        <v>44261</v>
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="e">
+        <f>DATEVALUE(2/3/2022)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>17</v>
@@ -625,21 +664,22 @@
         <v>30000</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="3">
-        <v>33124</v>
+        <v>26</v>
+      </c>
+      <c r="N3" s="3" t="e">
+        <f>DATEVALUE(10/13/1993)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D4" s="1">
         <v>123456</v>
@@ -648,13 +688,14 @@
         <v>9087634324</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="3">
-        <v>44622</v>
+        <v>24</v>
+      </c>
+      <c r="H4" s="3" t="e">
+        <f>DATEVALUE(2/3/2022)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>17</v>
@@ -663,21 +704,22 @@
         <v>12000</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="3">
-        <v>36046</v>
+        <v>32</v>
+      </c>
+      <c r="N4" s="3" t="e">
+        <f>DATEVALUE(11/22/1998)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D5" s="1">
         <v>123456</v>
@@ -686,13 +728,14 @@
         <v>9087655324</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="3">
-        <v>44780</v>
+        <v>24</v>
+      </c>
+      <c r="H5" s="3" t="e">
+        <f>DATEVALUE(2/3/2022)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>17</v>
@@ -701,19 +744,83 @@
         <v>12000</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="3" t="e">
+        <f>DATEVALUE(11/16/1995)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="3">
-        <v>34585</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="B6" s="2"/>
-      <c r="H6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="1">
+        <v>123456</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9456434855</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="3" t="e">
+        <f>DATEVALUE(2/3/2022)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="1">
+        <v>52000</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="3" t="e">
+        <f>DATEVALUE(11/23/1997)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="B7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9756484554</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="H7" s="3"/>
+      <c r="I7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="1">
+        <v>52000</v>
+      </c>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:15">
       <c r="B8" s="2"/>
@@ -877,8 +984,12 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="D7" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>